<commit_message>
Added sprint iteration plans
</commit_message>
<xml_diff>
--- a/Documentation/Burndown charts.xlsx
+++ b/Documentation/Burndown charts.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Amine's Stuff\programming\Android\Github\team01-Project\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harshil\Desktop\team01-Project-master\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17976" windowHeight="5940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10800"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="58">
   <si>
     <t>Task</t>
   </si>
@@ -153,6 +153,51 @@
   </si>
   <si>
     <t>Completed(6 sp)</t>
+  </si>
+  <si>
+    <t>Task 91</t>
+  </si>
+  <si>
+    <t>Task 92</t>
+  </si>
+  <si>
+    <t>Task 93</t>
+  </si>
+  <si>
+    <t>Task 94</t>
+  </si>
+  <si>
+    <t>Task 95</t>
+  </si>
+  <si>
+    <t>Task 96</t>
+  </si>
+  <si>
+    <t>Task 97</t>
+  </si>
+  <si>
+    <t>Estimated SP</t>
+  </si>
+  <si>
+    <t>Actual Remaning SP</t>
+  </si>
+  <si>
+    <t>Story Points</t>
+  </si>
+  <si>
+    <t>Completed(3 sp)</t>
+  </si>
+  <si>
+    <t>Task 103</t>
+  </si>
+  <si>
+    <t>Task 104</t>
+  </si>
+  <si>
+    <t>Task 105</t>
+  </si>
+  <si>
+    <t>Task 106</t>
   </si>
 </sst>
 </file>
@@ -1687,7 +1732,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10333733117797361"/>
+          <c:y val="0.17468311590921265"/>
+          <c:w val="0.89666266882202639"/>
+          <c:h val="0.67727759679390731"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -2299,6 +2354,946 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Sprint</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> 5 Burndown</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-CA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.7721372793161595E-2"/>
+          <c:y val="0.13297731239270383"/>
+          <c:w val="0.9304615727646014"/>
+          <c:h val="0.73086289762176759"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$64:$I$64</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Day 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$73:$I$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BDEE-48F7-B013-4BD38A371F28}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$64:$I$64</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Day 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$74:$I$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BDEE-48F7-B013-4BD38A371F28}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="300008304"/>
+        <c:axId val="300009288"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="300008304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="300009288"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="300009288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="300008304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Sprint</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> 6 Burndown</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-CA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Estimated</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$80:$I$80</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Day 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$89:$I$89</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-042A-42FA-8F9F-F2019E18A690}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Actual</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$80:$I$80</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Day 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$90:$I$90</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-042A-42FA-8F9F-F2019E18A690}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="348082696"/>
+        <c:axId val="346565032"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="348082696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="346565032"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="346565032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="348082696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2419,6 +3414,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -3614,6 +4689,1012 @@
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4031,16 +6112,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>198120</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>321945</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:rowOff>156210</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>434340</xdr:colOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>520065</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:rowOff>72390</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4054,6 +6135,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>481013</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4359,24 +6500,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H84" sqref="H84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="6" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.6640625" customWidth="1"/>
+    <col min="8" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -4408,7 +6549,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -4440,7 +6581,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -4472,7 +6613,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -4504,7 +6645,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -4536,7 +6677,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -4565,7 +6706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -4594,8 +6735,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:10" ht="32.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:10" ht="32.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -4627,7 +6768,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -4656,7 +6797,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -4685,13 +6826,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -4717,7 +6858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -4743,9 +6884,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -4777,7 +6918,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -4803,7 +6944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -4829,7 +6970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -4855,7 +6996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -4881,7 +7022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -4904,13 +7045,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -4936,7 +7077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -4962,13 +7103,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>29</v>
       </c>
@@ -5000,7 +7141,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -5032,7 +7173,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>18</v>
       </c>
@@ -5064,7 +7205,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -5096,7 +7237,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -5128,7 +7269,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>20</v>
       </c>
@@ -5160,7 +7301,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>34</v>
       </c>
@@ -5189,7 +7330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>13</v>
       </c>
@@ -5218,12 +7359,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>29</v>
       </c>
@@ -5255,7 +7396,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -5287,7 +7428,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>21</v>
       </c>
@@ -5319,7 +7460,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>23</v>
       </c>
@@ -5351,7 +7492,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>24</v>
       </c>
@@ -5383,7 +7524,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>22</v>
       </c>
@@ -5415,7 +7556,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -5447,7 +7588,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -5479,7 +7620,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>34</v>
       </c>
@@ -5508,7 +7649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>13</v>
       </c>
@@ -5534,6 +7675,532 @@
         <v>18</v>
       </c>
       <c r="I59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>52</v>
+      </c>
+      <c r="C64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" t="s">
+        <v>7</v>
+      </c>
+      <c r="F64" t="s">
+        <v>8</v>
+      </c>
+      <c r="G64" t="s">
+        <v>9</v>
+      </c>
+      <c r="H64" t="s">
+        <v>10</v>
+      </c>
+      <c r="I64" t="s">
+        <v>11</v>
+      </c>
+      <c r="J64" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>43</v>
+      </c>
+      <c r="B65">
+        <v>5</v>
+      </c>
+      <c r="C65">
+        <v>5</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>44</v>
+      </c>
+      <c r="B66">
+        <v>3</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>3</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>45</v>
+      </c>
+      <c r="B67">
+        <v>4</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>4</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>46</v>
+      </c>
+      <c r="B68">
+        <v>5</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>5</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+      <c r="J68" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>47</v>
+      </c>
+      <c r="B69">
+        <v>3</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>3</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="J69" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>48</v>
+      </c>
+      <c r="B70">
+        <v>5</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>5</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>49</v>
+      </c>
+      <c r="B71">
+        <v>4</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>4</v>
+      </c>
+      <c r="J71" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>50</v>
+      </c>
+      <c r="B73">
+        <v>29</v>
+      </c>
+      <c r="C73">
+        <v>29</v>
+      </c>
+      <c r="D73">
+        <v>24</v>
+      </c>
+      <c r="E73">
+        <v>19</v>
+      </c>
+      <c r="F73">
+        <v>14</v>
+      </c>
+      <c r="G73">
+        <v>9</v>
+      </c>
+      <c r="H73">
+        <v>4</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>51</v>
+      </c>
+      <c r="B74">
+        <v>29</v>
+      </c>
+      <c r="C74">
+        <v>24</v>
+      </c>
+      <c r="D74">
+        <v>21</v>
+      </c>
+      <c r="E74">
+        <v>17</v>
+      </c>
+      <c r="F74">
+        <v>12</v>
+      </c>
+      <c r="G74">
+        <v>7</v>
+      </c>
+      <c r="H74">
+        <v>4</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>52</v>
+      </c>
+      <c r="C80" t="s">
+        <v>5</v>
+      </c>
+      <c r="D80" t="s">
+        <v>6</v>
+      </c>
+      <c r="E80" t="s">
+        <v>7</v>
+      </c>
+      <c r="F80" t="s">
+        <v>8</v>
+      </c>
+      <c r="G80" t="s">
+        <v>9</v>
+      </c>
+      <c r="H80" t="s">
+        <v>10</v>
+      </c>
+      <c r="I80" t="s">
+        <v>11</v>
+      </c>
+      <c r="J80" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>54</v>
+      </c>
+      <c r="B81">
+        <v>5</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>5</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81">
+        <v>0</v>
+      </c>
+      <c r="J81" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>55</v>
+      </c>
+      <c r="B82">
+        <v>8</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>8</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82">
+        <v>0</v>
+      </c>
+      <c r="J82" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>56</v>
+      </c>
+      <c r="B83">
+        <v>6</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>6</v>
+      </c>
+      <c r="H83">
+        <v>0</v>
+      </c>
+      <c r="I83">
+        <v>0</v>
+      </c>
+      <c r="J83" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>57</v>
+      </c>
+      <c r="B84">
+        <v>5</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
+      </c>
+      <c r="I84">
+        <v>5</v>
+      </c>
+      <c r="J84" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>50</v>
+      </c>
+      <c r="B89">
+        <v>24</v>
+      </c>
+      <c r="C89">
+        <v>21</v>
+      </c>
+      <c r="D89">
+        <v>18</v>
+      </c>
+      <c r="E89">
+        <v>15</v>
+      </c>
+      <c r="F89">
+        <v>12</v>
+      </c>
+      <c r="G89">
+        <v>9</v>
+      </c>
+      <c r="H89">
+        <v>6</v>
+      </c>
+      <c r="I89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>51</v>
+      </c>
+      <c r="B90">
+        <v>24</v>
+      </c>
+      <c r="C90">
+        <v>24</v>
+      </c>
+      <c r="D90">
+        <v>24</v>
+      </c>
+      <c r="E90">
+        <v>11</v>
+      </c>
+      <c r="F90">
+        <v>11</v>
+      </c>
+      <c r="G90">
+        <v>5</v>
+      </c>
+      <c r="H90">
+        <v>5</v>
+      </c>
+      <c r="I90">
         <v>0</v>
       </c>
     </row>

</xml_diff>